<commit_message>
Updated 5-07-2019 -Part 1
</commit_message>
<xml_diff>
--- a/Data Files/TestData/Comission.xlsx
+++ b/Data Files/TestData/Comission.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20310" windowHeight="8325"/>
+    <workbookView windowWidth="20310" windowHeight="8325" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="MGA" sheetId="1" r:id="rId1"/>
     <sheet name="Insurer" sheetId="2" r:id="rId2"/>
     <sheet name="Broker" sheetId="3" r:id="rId3"/>
     <sheet name="MGATrialBalance" sheetId="4" r:id="rId4"/>
+    <sheet name="InsurerCommission" sheetId="5" r:id="rId5"/>
+    <sheet name="ExpectedBrokerComission" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="0">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="0">
   <si>
     <t>MGA Comission</t>
   </si>
@@ -28,13 +30,13 @@
     <t>Insurer Comission</t>
   </si>
   <si>
-    <t>84.00</t>
-  </si>
-  <si>
     <t>BrokerComission</t>
   </si>
   <si>
     <t>90.00</t>
+  </si>
+  <si>
+    <t>InsurerComission</t>
   </si>
 </sst>
 </file>
@@ -57,14 +59,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -216,25 +218,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -246,157 +398,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -510,7 +512,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -528,31 +530,31 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -570,22 +572,22 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -594,69 +596,70 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -976,15 +979,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.1428571428571" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="16.1428571428571" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -994,11 +997,6 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1014,12 +1012,12 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.2857142857143" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="18.2857142857143" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1028,8 +1026,8 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="A2" s="1">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1044,23 +1042,23 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.4285714285714" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="17.4285714285714" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="29.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1075,12 +1073,12 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.8571428571429" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="19.8571428571429" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1093,34 +1091,56 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>1</v>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="21.5714285714286" collapsed="false"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>1</v>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1">
+        <v>84</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>1</v>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>